<commit_message>
Udacity Front End Web Developer Nanodegree resources added.
</commit_message>
<xml_diff>
--- a/Front End Web Developer.xlsx
+++ b/Front End Web Developer.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4A1B3E-DA8C-4C51-8E91-4FC6089CD964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEABC4A-92E1-4C45-9916-DCC494E1C514}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Nano Degree" sheetId="2" r:id="rId2"/>
+    <sheet name="Front-End Master" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>https://www.udacity.com/course/intro-to-html-and-css--ud001</t>
   </si>
@@ -97,19 +99,154 @@
   </si>
   <si>
     <t>https://www.udacity.com/course/javascript-testing--ud549</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/web-development-v2/</t>
+  </si>
+  <si>
+    <t>Complete Intro to Web Development, v2</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/css-in-depth-v2/</t>
+  </si>
+  <si>
+    <t>CSS In-Depth, v2</t>
+  </si>
+  <si>
+    <t>CSS Grids and Flexbox for Responsive Web Design</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/css-grids-flexbox/</t>
+  </si>
+  <si>
+    <t>Advanced CSS Layouts</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/advanced-css-layouts/</t>
+  </si>
+  <si>
+    <t>https://classroom.udacity.com/nanodegrees/nd0011/dashboard/overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front End Web Developer  </t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/webpack-fundamentals/</t>
+  </si>
+  <si>
+    <t>Webpack 4 Fundamentals</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/performance-webpack/</t>
+  </si>
+  <si>
+    <t>Web Performance with Webpack</t>
+  </si>
+  <si>
+    <t>Webpack Plugins System</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/webpack-plugins/</t>
+  </si>
+  <si>
+    <t>Sass Fundamentals</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/sass/</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/secure-auth-jwt/</t>
+  </si>
+  <si>
+    <t>Secure Authentication for Web Apps &amp; APIs Using JWTs</t>
+  </si>
+  <si>
+    <t>Digging Into Node.js</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/digging-into-node/</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/workshops/dev-tools-v3/</t>
+  </si>
+  <si>
+    <t>Introduction to Dev Tools, v3</t>
+  </si>
+  <si>
+    <t>JavaScript Performance</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/web-performance/</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/typescript-v2/</t>
+  </si>
+  <si>
+    <t>TypeScript 3 Fundamentals, v2</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/javascript-hard-parts-v2/</t>
+  </si>
+  <si>
+    <t>JavaScript: The Hard Parts, v2</t>
+  </si>
+  <si>
+    <t>26 module</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/responsive-typography-v2/</t>
+  </si>
+  <si>
+    <t>Responsive Web Typography v2</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/html-email-v2/</t>
+  </si>
+  <si>
+    <t>HTML Email Development, v2</t>
+  </si>
+  <si>
+    <t>Introduction to Next.js</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/next-js/</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/production-next/</t>
+  </si>
+  <si>
+    <t>Production-Grade Next.js</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/modern-seo/</t>
+  </si>
+  <si>
+    <t>Modern Search Engine Optimization (SEO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F2932"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,8 +269,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BED189A-CD69-466C-96BE-A1C2D9787ACE}">
   <dimension ref="B2:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -559,4 +703,235 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4CA592-4195-4E9F-B368-BE7610B4C187}">
+  <dimension ref="B2:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="88.88671875" customWidth="1"/>
+    <col min="3" max="3" width="80.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F805ABA7-3AFC-402F-AE02-1E34EF41F5AF}">
+  <dimension ref="B2:C38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="88.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Google and MDN Resourses added.
</commit_message>
<xml_diff>
--- a/Front End Web Developer.xlsx
+++ b/Front End Web Developer.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEABC4A-92E1-4C45-9916-DCC494E1C514}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B0CFFF-565E-496C-BBF9-68D5D4804240}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Nano Degree" sheetId="2" r:id="rId2"/>
     <sheet name="Front-End Master" sheetId="3" r:id="rId3"/>
+    <sheet name="MDN" sheetId="4" r:id="rId4"/>
+    <sheet name="Google" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>https://www.udacity.com/course/intro-to-html-and-css--ud001</t>
   </si>
@@ -222,6 +224,45 @@
   </si>
   <si>
     <t>Modern Search Engine Optimization (SEO)</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTML</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTML/Element/button</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTML/Element/figure</t>
+  </si>
+  <si>
+    <t>Figure</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTML/Element</t>
+  </si>
+  <si>
+    <t>HTML Reference</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/CSS/Pseudo-classes</t>
+  </si>
+  <si>
+    <t>Pseudo Classes CSS</t>
+  </si>
+  <si>
+    <t>https://www.chromestatus.com/samples</t>
+  </si>
+  <si>
+    <t>Chrome Samples</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/web/fundamentals</t>
+  </si>
+  <si>
+    <t>Web Fundamentals</t>
   </si>
 </sst>
 </file>
@@ -741,7 +782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F805ABA7-3AFC-402F-AE02-1E34EF41F5AF}">
   <dimension ref="B2:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -934,4 +975,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28EBA50-CC43-4237-806F-603F4A2F4782}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="89.109375" customWidth="1"/>
+    <col min="3" max="3" width="88.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1714DA-44B5-4B61-BA25-71CC2B2533A1}">
+  <dimension ref="B2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="62.109375" customWidth="1"/>
+    <col min="3" max="3" width="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New MDN resources on Flexbox added. Some google and frontmaster courses added.
</commit_message>
<xml_diff>
--- a/Front End Web Developer.xlsx
+++ b/Front End Web Developer.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B0CFFF-565E-496C-BBF9-68D5D4804240}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D68B046-9BBC-4B1D-AA3A-AC1600852678}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Nano Degree" sheetId="2" r:id="rId2"/>
-    <sheet name="Front-End Master" sheetId="3" r:id="rId3"/>
-    <sheet name="MDN" sheetId="4" r:id="rId4"/>
-    <sheet name="Google" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="Nano Degree" sheetId="2" r:id="rId3"/>
+    <sheet name="Front-End Master" sheetId="3" r:id="rId4"/>
+    <sheet name="MDN" sheetId="4" r:id="rId5"/>
+    <sheet name="Frontend Master" sheetId="7" r:id="rId6"/>
+    <sheet name="CSS Tricks" sheetId="8" r:id="rId7"/>
+    <sheet name="Google" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>https://www.udacity.com/course/intro-to-html-and-css--ud001</t>
   </si>
@@ -263,13 +266,55 @@
   </si>
   <si>
     <t>Web Fundamentals</t>
+  </si>
+  <si>
+    <t>https://web.mit.edu/jmorzins/www/fonts.html</t>
+  </si>
+  <si>
+    <t>MIT Font</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/CSS/background-image</t>
+  </si>
+  <si>
+    <t>Background Images</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Learn/CSS/CSS_layout/Flexbox</t>
+  </si>
+  <si>
+    <t>Flexbox</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/CSS/CSS_Flexible_Box_Layout/Basic_Concepts_of_Flexbox</t>
+  </si>
+  <si>
+    <t>Flexbox Basic Concept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firebase with React, v2 </t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/courses/firebase-react-v2</t>
+  </si>
+  <si>
+    <t>https://css-tricks.com/firebase-crash-course/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firebase Crash Course </t>
+  </si>
+  <si>
+    <t>https://fonts.google.com/</t>
+  </si>
+  <si>
+    <t>Google Fonts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +332,13 @@
       <sz val="11"/>
       <color rgb="FF1F2932"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lato"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -310,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -318,6 +370,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,6 +802,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC092D8B-1D58-4EFD-B0BF-9C358A6EAC2E}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="62.44140625" customWidth="1"/>
+    <col min="3" max="3" width="71.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4CA592-4195-4E9F-B368-BE7610B4C187}">
   <dimension ref="B2:C6"/>
   <sheetViews>
@@ -778,7 +860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F805ABA7-3AFC-402F-AE02-1E34EF41F5AF}">
   <dimension ref="B2:C38"/>
   <sheetViews>
@@ -977,12 +1059,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28EBA50-CC43-4237-806F-603F4A2F4782}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,14 +1110,93 @@
         <v>72</v>
       </c>
     </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E0481D-A145-4A4E-88D0-911F64361480}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="62" customWidth="1"/>
+    <col min="3" max="3" width="115.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA4AD22-2256-4201-9AFE-46FCA2D6D2B8}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="62.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1714DA-44B5-4B61-BA25-71CC2B2533A1}">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1063,6 +1224,14 @@
         <v>76</v>
       </c>
     </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added some tools 	-> CSS Grid Generator 	-> Chrome Dev Tools link 	-> Grid v/s Flexbox articles
</commit_message>
<xml_diff>
--- a/Front End Web Developer.xlsx
+++ b/Front End Web Developer.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D68B046-9BBC-4B1D-AA3A-AC1600852678}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E028E389-1CB5-4BE0-8A92-1D9226A0D5A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="Blogs" sheetId="6" r:id="rId2"/>
     <sheet name="Nano Degree" sheetId="2" r:id="rId3"/>
     <sheet name="Front-End Master" sheetId="3" r:id="rId4"/>
     <sheet name="MDN" sheetId="4" r:id="rId5"/>
     <sheet name="Frontend Master" sheetId="7" r:id="rId6"/>
     <sheet name="CSS Tricks" sheetId="8" r:id="rId7"/>
-    <sheet name="Google" sheetId="5" r:id="rId8"/>
+    <sheet name="Tools" sheetId="9" r:id="rId8"/>
+    <sheet name="Google" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
   <si>
     <t>https://www.udacity.com/course/intro-to-html-and-css--ud001</t>
   </si>
@@ -308,13 +309,43 @@
   </si>
   <si>
     <t>Google Fonts</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/web/tools/chrome-devtools/</t>
+  </si>
+  <si>
+    <t>Chrome Dev-Tools</t>
+  </si>
+  <si>
+    <t>https://medium.com/youstart-labs/beginners-guide-to-choose-between-css-grid-and-flexbox-783005dd2412</t>
+  </si>
+  <si>
+    <t>Grid v/s Flexbox</t>
+  </si>
+  <si>
+    <t>https://hackernoon.com/the-ultimate-css-battle-grid-vs-flexbox-d40da0449faf</t>
+  </si>
+  <si>
+    <t>https://css-tricks.com/css-grid-replace-flexbox/</t>
+  </si>
+  <si>
+    <t>https://cssgrid-generator.netlify.app/</t>
+  </si>
+  <si>
+    <t>Grid Generator</t>
+  </si>
+  <si>
+    <t>https://github.com/sdras/cssgridgenerator</t>
+  </si>
+  <si>
+    <t>Grid Generator Source Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +372,13 @@
       <name val="Lato"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -374,6 +412,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,16 +842,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC092D8B-1D58-4EFD-B0BF-9C358A6EAC2E}">
-  <dimension ref="B2:C2"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="3" max="3" width="71.109375" customWidth="1"/>
+    <col min="3" max="3" width="116.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
@@ -821,6 +860,22 @@
       </c>
       <c r="C2" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1169,7 +1224,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA4AD22-2256-4201-9AFE-46FCA2D6D2B8}">
-  <dimension ref="B2:C2"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -1189,17 +1244,60 @@
         <v>88</v>
       </c>
     </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1714DA-44B5-4B61-BA25-71CC2B2533A1}">
-  <dimension ref="B2:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ACF5E0-9D1A-49DC-96A5-9B3788624172}">
+  <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="62.109375" customWidth="1"/>
+    <col min="3" max="3" width="115.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1714DA-44B5-4B61-BA25-71CC2B2533A1}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,6 +1330,14 @@
         <v>90</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Resources related to css grid added.
</commit_message>
<xml_diff>
--- a/Front End Web Developer.xlsx
+++ b/Front End Web Developer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E028E389-1CB5-4BE0-8A92-1D9226A0D5A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DF9E8A-5950-4394-8E54-177885469128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>https://www.udacity.com/course/intro-to-html-and-css--ud001</t>
   </si>
@@ -339,6 +339,48 @@
   </si>
   <si>
     <t>Grid Generator Source Code</t>
+  </si>
+  <si>
+    <t>https://mastery.games/post/grid-item-placement/</t>
+  </si>
+  <si>
+    <t>How Items Flows into CSS Grid</t>
+  </si>
+  <si>
+    <t>https://rachelandrew.co.uk/archives/2015/02/04/css-grid-layout-creating-complex-grids/</t>
+  </si>
+  <si>
+    <t>CSS Grid Layout - Creating Complex Grid</t>
+  </si>
+  <si>
+    <t>https://gridbyexample.com/examples/example21/</t>
+  </si>
+  <si>
+    <t>Nested Grid</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/CSS/Viewport_concepts#what_is_a_viewport</t>
+  </si>
+  <si>
+    <t>ViewPort Concept</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Mozilla/Mobile/Viewport_meta_tag</t>
+  </si>
+  <si>
+    <t>ViewPort meta tag</t>
+  </si>
+  <si>
+    <t>https://css-tricks.com/snippets/css/complete-guide-grid/</t>
+  </si>
+  <si>
+    <t>A Complete Guide to Grid</t>
+  </si>
+  <si>
+    <t>https://github.com/StartBootstrap/startbootstrap-grayscale</t>
+  </si>
+  <si>
+    <t>https://startbootstrap.com/</t>
   </si>
 </sst>
 </file>
@@ -842,10 +884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC092D8B-1D58-4EFD-B0BF-9C358A6EAC2E}">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,6 +918,54 @@
       </c>
       <c r="C6" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1259,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ACF5E0-9D1A-49DC-96A5-9B3788624172}">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1285,6 +1375,16 @@
       </c>
       <c r="C4" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resources on CSS grid and Flexbox added.
</commit_message>
<xml_diff>
--- a/Front End Web Developer.xlsx
+++ b/Front End Web Developer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DF9E8A-5950-4394-8E54-177885469128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39933D96-90A1-4AD1-848C-88EA74013F15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="9" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="Nano Degree" sheetId="2" r:id="rId3"/>
     <sheet name="Front-End Master" sheetId="3" r:id="rId4"/>
     <sheet name="MDN" sheetId="4" r:id="rId5"/>
-    <sheet name="Frontend Master" sheetId="7" r:id="rId6"/>
-    <sheet name="CSS Tricks" sheetId="8" r:id="rId7"/>
-    <sheet name="Tools" sheetId="9" r:id="rId8"/>
-    <sheet name="Google" sheetId="5" r:id="rId9"/>
+    <sheet name="W3School" sheetId="10" r:id="rId6"/>
+    <sheet name="Frontend Master" sheetId="7" r:id="rId7"/>
+    <sheet name="CSS Tricks" sheetId="8" r:id="rId8"/>
+    <sheet name="Tools" sheetId="9" r:id="rId9"/>
+    <sheet name="Google" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
   <si>
     <t>https://www.udacity.com/course/intro-to-html-and-css--ud001</t>
   </si>
@@ -381,6 +382,48 @@
   </si>
   <si>
     <t>https://startbootstrap.com/</t>
+  </si>
+  <si>
+    <t>https://css-tricks.com/snippets/css/a-guide-to-flexbox/</t>
+  </si>
+  <si>
+    <t>A complete guide to flexbox</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/CSS/CSS_Box_Model</t>
+  </si>
+  <si>
+    <t>CSS Box Model</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Learn/CSS/Building_blocks/The_box_model</t>
+  </si>
+  <si>
+    <t>The Box Model</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/css/css_rwd_intro.asp</t>
+  </si>
+  <si>
+    <t>Responsive Web Design</t>
+  </si>
+  <si>
+    <t>https://css-tricks.com/pseudo-class-selectors/</t>
+  </si>
+  <si>
+    <t>Pseudo Class Selector</t>
+  </si>
+  <si>
+    <t>https://css-tricks.com/almanac/selectors/a/after-and-before/</t>
+  </si>
+  <si>
+    <t>::before / ::after</t>
+  </si>
+  <si>
+    <t>https://www.paulirish.com/2012/box-sizing-border-box-ftw/</t>
+  </si>
+  <si>
+    <t>Border-Box property</t>
   </si>
 </sst>
 </file>
@@ -882,6 +925,65 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1714DA-44B5-4B61-BA25-71CC2B2533A1}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="62.109375" customWidth="1"/>
+    <col min="3" max="3" width="89" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC092D8B-1D58-4EFD-B0BF-9C358A6EAC2E}">
   <dimension ref="B2:C18"/>
@@ -1206,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28EBA50-CC43-4237-806F-603F4A2F4782}">
-  <dimension ref="B2:C16"/>
+  <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1279,12 +1381,55 @@
         <v>84</v>
       </c>
     </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23C98EC-E171-46FC-ABBB-543E260E7046}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
+    <col min="3" max="3" width="97.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E0481D-A145-4A4E-88D0-911F64361480}">
   <dimension ref="B2:C2"/>
   <sheetViews>
@@ -1312,12 +1457,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA4AD22-2256-4201-9AFE-46FCA2D6D2B8}">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,16 +1487,40 @@
         <v>97</v>
       </c>
     </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ACF5E0-9D1A-49DC-96A5-9B3788624172}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1390,55 +1559,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1714DA-44B5-4B61-BA25-71CC2B2533A1}">
-  <dimension ref="B2:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="62.109375" customWidth="1"/>
-    <col min="3" max="3" width="89" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added few articles and courses from egghead.
</commit_message>
<xml_diff>
--- a/Front End Web Developer.xlsx
+++ b/Front End Web Developer.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Excecl Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39933D96-90A1-4AD1-848C-88EA74013F15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A736387-7116-43E5-A1BF-992114BF53B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="9" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DB0C3086-B1D2-420C-8436-F4D5E53EF835}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blogs" sheetId="6" r:id="rId2"/>
-    <sheet name="Nano Degree" sheetId="2" r:id="rId3"/>
-    <sheet name="Front-End Master" sheetId="3" r:id="rId4"/>
-    <sheet name="MDN" sheetId="4" r:id="rId5"/>
-    <sheet name="W3School" sheetId="10" r:id="rId6"/>
-    <sheet name="Frontend Master" sheetId="7" r:id="rId7"/>
-    <sheet name="CSS Tricks" sheetId="8" r:id="rId8"/>
-    <sheet name="Tools" sheetId="9" r:id="rId9"/>
-    <sheet name="Google" sheetId="5" r:id="rId10"/>
+    <sheet name="Egghead" sheetId="11" r:id="rId2"/>
+    <sheet name="Blogs" sheetId="6" r:id="rId3"/>
+    <sheet name="Nano Degree" sheetId="2" r:id="rId4"/>
+    <sheet name="Front-End Master" sheetId="3" r:id="rId5"/>
+    <sheet name="MDN" sheetId="4" r:id="rId6"/>
+    <sheet name="W3School" sheetId="10" r:id="rId7"/>
+    <sheet name="Frontend Master" sheetId="7" r:id="rId8"/>
+    <sheet name="CSS Tricks" sheetId="8" r:id="rId9"/>
+    <sheet name="Tools" sheetId="9" r:id="rId10"/>
+    <sheet name="Google" sheetId="5" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="144">
   <si>
     <t>https://www.udacity.com/course/intro-to-html-and-css--ud001</t>
   </si>
@@ -424,6 +425,48 @@
   </si>
   <si>
     <t>Border-Box property</t>
+  </si>
+  <si>
+    <t>https://github.com/FrontendMasters/learning-roadmap</t>
+  </si>
+  <si>
+    <t>Frontend Master Roadmap</t>
+  </si>
+  <si>
+    <t>https://mastery.games/flexboxzombies/</t>
+  </si>
+  <si>
+    <t>Flexbox Zombies</t>
+  </si>
+  <si>
+    <t>https://flexboxfroggy.com/</t>
+  </si>
+  <si>
+    <t>Flexbox Froggy</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/CSS/Media_Queries/Using_media_queries</t>
+  </si>
+  <si>
+    <t>Media Queries</t>
+  </si>
+  <si>
+    <t>https://frontendmasters.com/guides/learning-roadmap/web-security/</t>
+  </si>
+  <si>
+    <t>Frontend Masters Web Security</t>
+  </si>
+  <si>
+    <t>https://egghead.io/courses/css-fundamentals</t>
+  </si>
+  <si>
+    <t>CSS Fundamental</t>
+  </si>
+  <si>
+    <t>https://egghead.io/courses/build-modern-layouts-with-css-grid-d3f5</t>
+  </si>
+  <si>
+    <t>Build modern layout with CSS Grid</t>
   </si>
 </sst>
 </file>
@@ -814,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BED189A-CD69-466C-96BE-A1C2D9787ACE}">
   <dimension ref="B2:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -926,10 +969,71 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ACF5E0-9D1A-49DC-96A5-9B3788624172}">
+  <dimension ref="B2:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="62.109375" customWidth="1"/>
+    <col min="3" max="3" width="115.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1714DA-44B5-4B61-BA25-71CC2B2533A1}">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -985,6 +1089,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E501919-19E2-4674-A4EA-67B1C82F7A62}">
+  <dimension ref="B2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="53.109375" customWidth="1"/>
+    <col min="3" max="3" width="97.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC092D8B-1D58-4EFD-B0BF-9C358A6EAC2E}">
   <dimension ref="B2:C18"/>
   <sheetViews>
@@ -1075,7 +1214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4CA592-4195-4E9F-B368-BE7610B4C187}">
   <dimension ref="B2:C6"/>
   <sheetViews>
@@ -1107,7 +1246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F805ABA7-3AFC-402F-AE02-1E34EF41F5AF}">
   <dimension ref="B2:C38"/>
   <sheetViews>
@@ -1306,9 +1445,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28EBA50-CC43-4237-806F-603F4A2F4782}">
-  <dimension ref="B2:C20"/>
+  <dimension ref="B2:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -1397,12 +1536,20 @@
         <v>120</v>
       </c>
     </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23C98EC-E171-46FC-ABBB-543E260E7046}">
   <dimension ref="B2:C2"/>
   <sheetViews>
@@ -1429,12 +1576,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E0481D-A145-4A4E-88D0-911F64361480}">
-  <dimension ref="B2:C2"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,18 +1598,34 @@
         <v>87</v>
       </c>
     </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA4AD22-2256-4201-9AFE-46FCA2D6D2B8}">
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1514,49 +1677,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ACF5E0-9D1A-49DC-96A5-9B3788624172}">
-  <dimension ref="B2:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="62.109375" customWidth="1"/>
-    <col min="3" max="3" width="115.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>